<commit_message>
GDE-9323 - added new base rate file for ATM BILAT
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD6CEEE-B2B4-44D6-9E1C-CD455744F64E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019A2780-1F3C-48F9-9B3E-DFE70B079383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="28800" windowHeight="7830" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>rowid</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20191218.csv</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20190921.csv</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +658,23 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{BC47C54F-DEBA-4A4C-B7BD-5C1F7EAEAC13}"/>
@@ -660,9 +683,11 @@
     <hyperlink ref="C4:C5" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{407C1BE7-9490-4661-BC30-07F9C1CD1B2C}"/>
     <hyperlink ref="D2" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4C02B099-3543-4FDE-A178-CD6D6DBBC63A}"/>
     <hyperlink ref="C2" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDA2A936-5571-40FB-ACD9-716945EE58E8}"/>
+    <hyperlink ref="D6" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1FEBEDA4-A8F6-4C12-9223-52C62F6A804E}"/>
+    <hyperlink ref="C6" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{91054E13-F530-43F8-897A-07580A2AEEAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feature/GDE-9268 updates for Base rate Dec312019 PIM Future BILAT
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0B1A1A-407F-4AE3-89D2-609AC52E37C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9505442E-9E52-43E0-B54E-D2DEE849ABA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>rowid</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20191216.csv</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_31DEC2019\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20191231.csv</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_31122019</t>
   </si>
 </sst>
 </file>
@@ -536,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +711,23 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{BC47C54F-DEBA-4A4C-B7BD-5C1F7EAEAC13}"/>
@@ -711,9 +740,11 @@
     <hyperlink ref="C6" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{91054E13-F530-43F8-897A-07580A2AEEAF}"/>
     <hyperlink ref="D7" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2E8EA7CD-A546-4721-91A5-240576566310}"/>
     <hyperlink ref="C7" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
+    <hyperlink ref="D8" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
+    <hyperlink ref="C8" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feature/GDE-9269 updates for base rate for PIM Future BILAT
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9505442E-9E52-43E0-B54E-D2DEE849ABA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA54FBF-A722-4D71-8045-39450F5467FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>rowid</t>
   </si>
@@ -115,13 +115,25 @@
   </si>
   <si>
     <t>01_TL_Base_Rates_31122019</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_31012020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_31JAN2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200131.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +172,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -548,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +746,25 @@
         <v>24</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{BC47C54F-DEBA-4A4C-B7BD-5C1F7EAEAC13}"/>
     <hyperlink ref="C3" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D4056747-E844-4D5C-90C1-5C11EC476849}"/>
@@ -742,9 +778,11 @@
     <hyperlink ref="C7" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
     <hyperlink ref="D8" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
     <hyperlink ref="C8" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
+    <hyperlink ref="C9" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
+    <hyperlink ref="D9" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feature/GDE-9274 Load BR 02072020 for PIM Future Bilat
Added new csv file for base rate for 02072020
Added new folder and test suite
Updated previous csv to have correct rates on correct file date
Updated Data set to add new base rate
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B7D373-5581-4C3C-A935-3FF9068E34D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588F24EE-B192-4181-AB23-A39A637F515C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-2730" windowWidth="29040" windowHeight="16440" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseRate_Fields" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>rowid</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_07022020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_07FEB2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200207.csv</t>
   </si>
   <si>
     <t>12</t>
@@ -624,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +899,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>28</v>
@@ -900,6 +912,23 @@
       </c>
       <c r="E13" s="9" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -927,9 +956,11 @@
     <hyperlink ref="D10" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{28D6E063-1A13-4EE4-9635-6B563297A460}"/>
     <hyperlink ref="D11" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4DF6CFC3-BDCF-4610-B062-0DBDD3BA2867}"/>
     <hyperlink ref="C11" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4BBE60E-ECDA-42CC-8227-1E0F590B6063}"/>
+    <hyperlink ref="C14" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
+    <hyperlink ref="D14" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GDE-9408 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588F24EE-B192-4181-AB23-A39A637F515C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2377526C-1318-4530-9A7A-68FFCA576C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
   <si>
     <t>rowid</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_03012020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_03JAN2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200103.csv</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -284,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,6 +332,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,36 +913,53 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -946,8 +978,8 @@
     <hyperlink ref="C7" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
     <hyperlink ref="D12" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
     <hyperlink ref="C12" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
-    <hyperlink ref="C13" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
-    <hyperlink ref="D13" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
+    <hyperlink ref="C14" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
+    <hyperlink ref="D14" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
     <hyperlink ref="D3" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5F24D8F4-ADA1-47AC-95D6-7968D6A09C50}"/>
     <hyperlink ref="C3" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6F4AE858-8863-4D89-9817-A612F222D040}"/>
     <hyperlink ref="D6" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1689072D-A1FB-4764-96D9-65D8022C4964}"/>
@@ -956,11 +988,13 @@
     <hyperlink ref="D10" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{28D6E063-1A13-4EE4-9635-6B563297A460}"/>
     <hyperlink ref="D11" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4DF6CFC3-BDCF-4610-B062-0DBDD3BA2867}"/>
     <hyperlink ref="C11" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4BBE60E-ECDA-42CC-8227-1E0F590B6063}"/>
-    <hyperlink ref="C14" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
-    <hyperlink ref="D14" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
+    <hyperlink ref="C15" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
+    <hyperlink ref="D15" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
+    <hyperlink ref="C13" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC5028D8-19EE-4A5D-8630-ADFFD353D502}"/>
+    <hyperlink ref="D13" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDDBAFB6-B333-490E-B77D-1C8743D3E12B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feature/GDE-9584 Base Rate 19022020 for PIM Future BILAT
Updated data set
Added new csv file for base rate
Added new test suite
rename New life test suite so that base rate will run first for
19-FEB-2020
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED4089-83D9-407A-9340-85B00E35F787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3B885E-31A5-4824-B5EE-4B653B913DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>rowid</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_15JAN2020\</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_19022020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_19FEB2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200219.csv</t>
   </si>
 </sst>
 </file>
@@ -663,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,6 +1002,23 @@
       </c>
       <c r="E16" s="9" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1023,9 +1052,11 @@
     <hyperlink ref="D13" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDDBAFB6-B333-490E-B77D-1C8743D3E12B}"/>
     <hyperlink ref="C16" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{45E8D193-08A6-4F4A-96EE-B54BBAB37372}"/>
     <hyperlink ref="D16" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5EE5A545-9714-41D3-876A-3D94B6DD87EA}"/>
+    <hyperlink ref="C17" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0BDC0653-E3A8-439B-B2B0-9D715294B0B8}"/>
+    <hyperlink ref="D17" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E273B7EF-844E-4766-B928-9979CFA5B572}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId29"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GDE-9412 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3B885E-31A5-4824-B5EE-4B653B913DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2378404-DAAA-43EF-821A-813E09EDEBA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,58 +953,58 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>51</v>
       </c>
@@ -1036,8 +1036,8 @@
     <hyperlink ref="C7" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
     <hyperlink ref="D12" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
     <hyperlink ref="C12" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
-    <hyperlink ref="C14" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
-    <hyperlink ref="D14" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
+    <hyperlink ref="C15" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
+    <hyperlink ref="D15" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
     <hyperlink ref="D3" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5F24D8F4-ADA1-47AC-95D6-7968D6A09C50}"/>
     <hyperlink ref="C3" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6F4AE858-8863-4D89-9817-A612F222D040}"/>
     <hyperlink ref="D6" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1689072D-A1FB-4764-96D9-65D8022C4964}"/>
@@ -1046,12 +1046,12 @@
     <hyperlink ref="D10" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{28D6E063-1A13-4EE4-9635-6B563297A460}"/>
     <hyperlink ref="D11" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4DF6CFC3-BDCF-4610-B062-0DBDD3BA2867}"/>
     <hyperlink ref="C11" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4BBE60E-ECDA-42CC-8227-1E0F590B6063}"/>
-    <hyperlink ref="C15" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
-    <hyperlink ref="D15" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
+    <hyperlink ref="C16" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
+    <hyperlink ref="D16" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
     <hyperlink ref="C13" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC5028D8-19EE-4A5D-8630-ADFFD353D502}"/>
     <hyperlink ref="D13" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDDBAFB6-B333-490E-B77D-1C8743D3E12B}"/>
-    <hyperlink ref="C16" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{45E8D193-08A6-4F4A-96EE-B54BBAB37372}"/>
-    <hyperlink ref="D16" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5EE5A545-9714-41D3-876A-3D94B6DD87EA}"/>
+    <hyperlink ref="C14" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{45E8D193-08A6-4F4A-96EE-B54BBAB37372}"/>
+    <hyperlink ref="D14" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5EE5A545-9714-41D3-876A-3D94B6DD87EA}"/>
     <hyperlink ref="C17" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0BDC0653-E3A8-439B-B2B0-9D715294B0B8}"/>
     <hyperlink ref="D17" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E273B7EF-844E-4766-B928-9979CFA5B572}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
GDE-9414 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACC6BDA-D834-4996-8944-96BEA7D580CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ECB30C-9FA9-4D65-9A95-9B42467B86D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>rowid</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200123.csv</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_03022020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_03FEB2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200203.csv</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -687,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,21 +994,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
@@ -1004,50 +1016,67 @@
         <v>47</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>58</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1065,8 +1094,8 @@
     <hyperlink ref="C7" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
     <hyperlink ref="D12" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
     <hyperlink ref="C12" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
-    <hyperlink ref="C15" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
-    <hyperlink ref="D15" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
+    <hyperlink ref="C16" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
+    <hyperlink ref="D16" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
     <hyperlink ref="D3" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5F24D8F4-ADA1-47AC-95D6-7968D6A09C50}"/>
     <hyperlink ref="C3" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6F4AE858-8863-4D89-9817-A612F222D040}"/>
     <hyperlink ref="D6" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1689072D-A1FB-4764-96D9-65D8022C4964}"/>
@@ -1075,19 +1104,21 @@
     <hyperlink ref="D10" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{28D6E063-1A13-4EE4-9635-6B563297A460}"/>
     <hyperlink ref="D11" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4DF6CFC3-BDCF-4610-B062-0DBDD3BA2867}"/>
     <hyperlink ref="C11" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4BBE60E-ECDA-42CC-8227-1E0F590B6063}"/>
-    <hyperlink ref="C16" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
-    <hyperlink ref="D16" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
+    <hyperlink ref="C18" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
+    <hyperlink ref="D18" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
     <hyperlink ref="C13" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC5028D8-19EE-4A5D-8630-ADFFD353D502}"/>
     <hyperlink ref="D13" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDDBAFB6-B333-490E-B77D-1C8743D3E12B}"/>
     <hyperlink ref="C14" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{45E8D193-08A6-4F4A-96EE-B54BBAB37372}"/>
     <hyperlink ref="D14" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5EE5A545-9714-41D3-876A-3D94B6DD87EA}"/>
-    <hyperlink ref="C17" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0BDC0653-E3A8-439B-B2B0-9D715294B0B8}"/>
-    <hyperlink ref="D17" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E273B7EF-844E-4766-B928-9979CFA5B572}"/>
-    <hyperlink ref="C18" r:id="rId31" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{25B9118A-8384-4480-8F25-36D9D388AB4C}"/>
-    <hyperlink ref="D18" r:id="rId32" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FB16881B-FC05-46D7-9BD2-DF33F0DC9095}"/>
+    <hyperlink ref="C19" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0BDC0653-E3A8-439B-B2B0-9D715294B0B8}"/>
+    <hyperlink ref="D19" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E273B7EF-844E-4766-B928-9979CFA5B572}"/>
+    <hyperlink ref="C15" r:id="rId31" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{25B9118A-8384-4480-8F25-36D9D388AB4C}"/>
+    <hyperlink ref="D15" r:id="rId32" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FB16881B-FC05-46D7-9BD2-DF33F0DC9095}"/>
+    <hyperlink ref="C17" r:id="rId33" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB9A20BF-0A23-49AB-A38C-A936AD770CD8}"/>
+    <hyperlink ref="D17" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E7ED670A-C93A-4D33-8D6B-C2A84F6272BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId33"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId35"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GDE-9535 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508EA344-0794-4CDE-B28D-71EBB345947E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC176D0-0F49-46AC-948D-C34CA23D0DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>rowid</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>01_TL_Base_Rates_31032020</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_24022020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_24FEB2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200224.csv</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -723,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,15 +1137,32 @@
         <v>67</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1176,11 +1205,13 @@
     <hyperlink ref="D17" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E7ED670A-C93A-4D33-8D6B-C2A84F6272BF}"/>
     <hyperlink ref="C19" r:id="rId35" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FEFD670A-BEB8-4A0B-98C5-2AFD4DEAD2BD}"/>
     <hyperlink ref="D19" r:id="rId36" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB25DD26-7137-4B60-8CDB-1EB5B00EE84D}"/>
-    <hyperlink ref="C21" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B18C013E-BB2E-4151-85B5-939674E1518A}"/>
-    <hyperlink ref="D21" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{681506BD-6C7D-465C-B4C1-2DE78EEE8983}"/>
+    <hyperlink ref="C22" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B18C013E-BB2E-4151-85B5-939674E1518A}"/>
+    <hyperlink ref="D22" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{681506BD-6C7D-465C-B4C1-2DE78EEE8983}"/>
+    <hyperlink ref="C21" r:id="rId39" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{439E8B61-D40D-4F84-B8BE-9700FC2ADD62}"/>
+    <hyperlink ref="D21" r:id="rId40" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5E6AC098-5E3E-4433-93A6-C293BACD8FDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId39"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId41"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GDE-9538 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u724659\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2FAEE-7EA2-41BF-9127-8C9F81B32B87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0466183F-50AE-4311-8A18-CDF1E91A12B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>rowid</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200316.csv</t>
+  </si>
+  <si>
+    <t>01_TL_Base_Rates_04032020</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_04MAR2020\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200304.csv</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
 </sst>
 </file>
@@ -747,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,37 +1173,54 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1234,15 +1263,17 @@
     <hyperlink ref="D17" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E7ED670A-C93A-4D33-8D6B-C2A84F6272BF}"/>
     <hyperlink ref="C19" r:id="rId35" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FEFD670A-BEB8-4A0B-98C5-2AFD4DEAD2BD}"/>
     <hyperlink ref="D19" r:id="rId36" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB25DD26-7137-4B60-8CDB-1EB5B00EE84D}"/>
-    <hyperlink ref="C23" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B18C013E-BB2E-4151-85B5-939674E1518A}"/>
-    <hyperlink ref="D23" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{681506BD-6C7D-465C-B4C1-2DE78EEE8983}"/>
+    <hyperlink ref="C24" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B18C013E-BB2E-4151-85B5-939674E1518A}"/>
+    <hyperlink ref="D24" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{681506BD-6C7D-465C-B4C1-2DE78EEE8983}"/>
     <hyperlink ref="C21" r:id="rId39" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{439E8B61-D40D-4F84-B8BE-9700FC2ADD62}"/>
     <hyperlink ref="D21" r:id="rId40" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5E6AC098-5E3E-4433-93A6-C293BACD8FDC}"/>
-    <hyperlink ref="C22" r:id="rId41" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6337C7C3-22E8-4713-B355-F29F547C2E90}"/>
-    <hyperlink ref="D22" r:id="rId42" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{61348313-29E4-410E-A720-44ABC90AACF2}"/>
+    <hyperlink ref="C23" r:id="rId41" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6337C7C3-22E8-4713-B355-F29F547C2E90}"/>
+    <hyperlink ref="D23" r:id="rId42" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{61348313-29E4-410E-A720-44ABC90AACF2}"/>
+    <hyperlink ref="C22" r:id="rId43" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{81D4A9F8-C5E5-4FB2-B5C6-66060C673A7C}"/>
+    <hyperlink ref="D22" r:id="rId44" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{79C6B99F-3134-484C-BF17-FF032736A4F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId43"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId45"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GDE-9331: pulled latest TL_Data_Set_New_UAT.xlsx and added my update on row 1. also updated rowid
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Data_Set_New_UAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\Transformation_Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278B52CC-C1E6-4841-AA3B-3DA2F0ECE010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67FAC14-A9EF-4297-9C4E-6BA66CF0A735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B57B0A42-B9E9-4F9A-A394-E95B8E00D96E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
   <si>
     <t>rowid</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20200415.csv</t>
+  </si>
+  <si>
+    <t>\DataSet\NewUATDeals_DataSet\Transformation_Layer\TL_Base_Rate\BaseRates_Files_04SEP2019\</t>
+  </si>
+  <si>
+    <t>FINASTRA_CCB_BASERATE_SY_GROUP1_20190904.csv</t>
+  </si>
+  <si>
+    <t>26</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -467,9 +476,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -786,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E7C826-6239-4631-B7A2-7901FE3648F4}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,10 +841,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -855,7 +861,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -878,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -901,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -924,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -947,7 +953,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -964,7 +970,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -987,7 +993,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1000,34 +1006,34 @@
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>35</v>
+      <c r="E10" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>36</v>
+      <c r="E11" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1035,315 +1041,334 @@
         <v>34</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="7" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="7" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="7" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="7" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="7" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="7" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="7" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="C25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E26" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="6" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="6" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{BC47C54F-DEBA-4A4C-B7BD-5C1F7EAEAC13}"/>
-    <hyperlink ref="C5" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D4056747-E844-4D5C-90C1-5C11EC476849}"/>
-    <hyperlink ref="D8:D9" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{39E7DDA4-AAF5-41BF-807B-8AC13C4EBB6E}"/>
-    <hyperlink ref="C8:C9" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{407C1BE7-9490-4661-BC30-07F9C1CD1B2C}"/>
-    <hyperlink ref="D4" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4C02B099-3543-4FDE-A178-CD6D6DBBC63A}"/>
-    <hyperlink ref="C4" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDA2A936-5571-40FB-ACD9-716945EE58E8}"/>
-    <hyperlink ref="D2" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1FEBEDA4-A8F6-4C12-9223-52C62F6A804E}"/>
-    <hyperlink ref="C2" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{91054E13-F530-43F8-897A-07580A2AEEAF}"/>
-    <hyperlink ref="D7" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2E8EA7CD-A546-4721-91A5-240576566310}"/>
-    <hyperlink ref="C7" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
-    <hyperlink ref="D12" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
-    <hyperlink ref="C12" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
-    <hyperlink ref="C16" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
-    <hyperlink ref="D16" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
-    <hyperlink ref="D3" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5F24D8F4-ADA1-47AC-95D6-7968D6A09C50}"/>
-    <hyperlink ref="C3" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6F4AE858-8863-4D89-9817-A612F222D040}"/>
-    <hyperlink ref="D6" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1689072D-A1FB-4764-96D9-65D8022C4964}"/>
-    <hyperlink ref="C6" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EBC0465F-D16C-46F0-B685-F68650E09CBE}"/>
-    <hyperlink ref="C10" r:id="rId19" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0FC5C92D-97AF-47F0-82A6-56F0027DD7CA}"/>
-    <hyperlink ref="D10" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{28D6E063-1A13-4EE4-9635-6B563297A460}"/>
-    <hyperlink ref="D11" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4DF6CFC3-BDCF-4610-B062-0DBDD3BA2867}"/>
-    <hyperlink ref="C11" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4BBE60E-ECDA-42CC-8227-1E0F590B6063}"/>
-    <hyperlink ref="C18" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
-    <hyperlink ref="D18" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
-    <hyperlink ref="C13" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC5028D8-19EE-4A5D-8630-ADFFD353D502}"/>
-    <hyperlink ref="D13" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDDBAFB6-B333-490E-B77D-1C8743D3E12B}"/>
-    <hyperlink ref="C14" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{45E8D193-08A6-4F4A-96EE-B54BBAB37372}"/>
-    <hyperlink ref="D14" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5EE5A545-9714-41D3-876A-3D94B6DD87EA}"/>
-    <hyperlink ref="C20" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0BDC0653-E3A8-439B-B2B0-9D715294B0B8}"/>
-    <hyperlink ref="D20" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E273B7EF-844E-4766-B928-9979CFA5B572}"/>
-    <hyperlink ref="C15" r:id="rId31" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{25B9118A-8384-4480-8F25-36D9D388AB4C}"/>
-    <hyperlink ref="D15" r:id="rId32" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FB16881B-FC05-46D7-9BD2-DF33F0DC9095}"/>
-    <hyperlink ref="C17" r:id="rId33" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB9A20BF-0A23-49AB-A38C-A936AD770CD8}"/>
-    <hyperlink ref="D17" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E7ED670A-C93A-4D33-8D6B-C2A84F6272BF}"/>
-    <hyperlink ref="C19" r:id="rId35" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FEFD670A-BEB8-4A0B-98C5-2AFD4DEAD2BD}"/>
-    <hyperlink ref="D19" r:id="rId36" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB25DD26-7137-4B60-8CDB-1EB5B00EE84D}"/>
-    <hyperlink ref="C25" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B18C013E-BB2E-4151-85B5-939674E1518A}"/>
-    <hyperlink ref="D25" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{681506BD-6C7D-465C-B4C1-2DE78EEE8983}"/>
-    <hyperlink ref="C21" r:id="rId39" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{439E8B61-D40D-4F84-B8BE-9700FC2ADD62}"/>
-    <hyperlink ref="D21" r:id="rId40" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5E6AC098-5E3E-4433-93A6-C293BACD8FDC}"/>
-    <hyperlink ref="C23" r:id="rId41" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6337C7C3-22E8-4713-B355-F29F547C2E90}"/>
-    <hyperlink ref="D23" r:id="rId42" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{61348313-29E4-410E-A720-44ABC90AACF2}"/>
-    <hyperlink ref="C22" r:id="rId43" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{81D4A9F8-C5E5-4FB2-B5C6-66060C673A7C}"/>
-    <hyperlink ref="D22" r:id="rId44" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{79C6B99F-3134-484C-BF17-FF032736A4F6}"/>
-    <hyperlink ref="C24" r:id="rId45" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F6E541ED-A56D-4990-98EC-140DB39C69BA}"/>
-    <hyperlink ref="D24" r:id="rId46" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A0CF9FAE-BAE8-4388-B3DA-F87DE7AAD9AE}"/>
-    <hyperlink ref="C26" r:id="rId47" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FE8FBBD9-8143-413A-8354-C1249A1B80F8}"/>
-    <hyperlink ref="D26" r:id="rId48" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{8C4BE03A-3602-4A55-A11A-8786FAAD6358}"/>
+    <hyperlink ref="D6" r:id="rId1" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{BC47C54F-DEBA-4A4C-B7BD-5C1F7EAEAC13}"/>
+    <hyperlink ref="C6" r:id="rId2" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D4056747-E844-4D5C-90C1-5C11EC476849}"/>
+    <hyperlink ref="D9:D10" r:id="rId3" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{39E7DDA4-AAF5-41BF-807B-8AC13C4EBB6E}"/>
+    <hyperlink ref="C9:C10" r:id="rId4" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{407C1BE7-9490-4661-BC30-07F9C1CD1B2C}"/>
+    <hyperlink ref="D5" r:id="rId5" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4C02B099-3543-4FDE-A178-CD6D6DBBC63A}"/>
+    <hyperlink ref="C5" r:id="rId6" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDA2A936-5571-40FB-ACD9-716945EE58E8}"/>
+    <hyperlink ref="D3" r:id="rId7" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1FEBEDA4-A8F6-4C12-9223-52C62F6A804E}"/>
+    <hyperlink ref="C3" r:id="rId8" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{91054E13-F530-43F8-897A-07580A2AEEAF}"/>
+    <hyperlink ref="D8" r:id="rId9" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{2E8EA7CD-A546-4721-91A5-240576566310}"/>
+    <hyperlink ref="C8" r:id="rId10" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D32611A9-A7C5-4DD4-BCCF-DA8133CD25B4}"/>
+    <hyperlink ref="D13" r:id="rId11" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{70815E86-B823-45F9-AC04-6D2D692DF861}"/>
+    <hyperlink ref="C13" r:id="rId12" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{3A752EAB-A2F0-4B6A-A66D-032CEEC610CE}"/>
+    <hyperlink ref="C17" r:id="rId13" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{D2AEB5F3-3204-4436-AD53-801A83DD4EBE}"/>
+    <hyperlink ref="D17" r:id="rId14" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EAD750A5-37C4-46A7-9B44-118A9975371E}"/>
+    <hyperlink ref="D4" r:id="rId15" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5F24D8F4-ADA1-47AC-95D6-7968D6A09C50}"/>
+    <hyperlink ref="C4" r:id="rId16" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6F4AE858-8863-4D89-9817-A612F222D040}"/>
+    <hyperlink ref="D7" r:id="rId17" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1689072D-A1FB-4764-96D9-65D8022C4964}"/>
+    <hyperlink ref="C7" r:id="rId18" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EBC0465F-D16C-46F0-B685-F68650E09CBE}"/>
+    <hyperlink ref="C11" r:id="rId19" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0FC5C92D-97AF-47F0-82A6-56F0027DD7CA}"/>
+    <hyperlink ref="D11" r:id="rId20" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{28D6E063-1A13-4EE4-9635-6B563297A460}"/>
+    <hyperlink ref="D12" r:id="rId21" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{4DF6CFC3-BDCF-4610-B062-0DBDD3BA2867}"/>
+    <hyperlink ref="C12" r:id="rId22" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B4BBE60E-ECDA-42CC-8227-1E0F590B6063}"/>
+    <hyperlink ref="C19" r:id="rId23" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A1392737-75BD-4B08-801B-426CE5631F3F}"/>
+    <hyperlink ref="D19" r:id="rId24" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{38D310A5-27BA-4A2A-B06F-99C45615013F}"/>
+    <hyperlink ref="C14" r:id="rId25" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{EC5028D8-19EE-4A5D-8630-ADFFD353D502}"/>
+    <hyperlink ref="D14" r:id="rId26" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FDDBAFB6-B333-490E-B77D-1C8743D3E12B}"/>
+    <hyperlink ref="C15" r:id="rId27" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{45E8D193-08A6-4F4A-96EE-B54BBAB37372}"/>
+    <hyperlink ref="D15" r:id="rId28" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5EE5A545-9714-41D3-876A-3D94B6DD87EA}"/>
+    <hyperlink ref="C21" r:id="rId29" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{0BDC0653-E3A8-439B-B2B0-9D715294B0B8}"/>
+    <hyperlink ref="D21" r:id="rId30" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E273B7EF-844E-4766-B928-9979CFA5B572}"/>
+    <hyperlink ref="C16" r:id="rId31" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{25B9118A-8384-4480-8F25-36D9D388AB4C}"/>
+    <hyperlink ref="D16" r:id="rId32" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FB16881B-FC05-46D7-9BD2-DF33F0DC9095}"/>
+    <hyperlink ref="C18" r:id="rId33" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB9A20BF-0A23-49AB-A38C-A936AD770CD8}"/>
+    <hyperlink ref="D18" r:id="rId34" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{E7ED670A-C93A-4D33-8D6B-C2A84F6272BF}"/>
+    <hyperlink ref="C20" r:id="rId35" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FEFD670A-BEB8-4A0B-98C5-2AFD4DEAD2BD}"/>
+    <hyperlink ref="D20" r:id="rId36" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{AB25DD26-7137-4B60-8CDB-1EB5B00EE84D}"/>
+    <hyperlink ref="C26" r:id="rId37" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{B18C013E-BB2E-4151-85B5-939674E1518A}"/>
+    <hyperlink ref="D26" r:id="rId38" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{681506BD-6C7D-465C-B4C1-2DE78EEE8983}"/>
+    <hyperlink ref="C22" r:id="rId39" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{439E8B61-D40D-4F84-B8BE-9700FC2ADD62}"/>
+    <hyperlink ref="D22" r:id="rId40" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{5E6AC098-5E3E-4433-93A6-C293BACD8FDC}"/>
+    <hyperlink ref="C24" r:id="rId41" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6337C7C3-22E8-4713-B355-F29F547C2E90}"/>
+    <hyperlink ref="D24" r:id="rId42" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{61348313-29E4-410E-A720-44ABC90AACF2}"/>
+    <hyperlink ref="C23" r:id="rId43" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{81D4A9F8-C5E5-4FB2-B5C6-66060C673A7C}"/>
+    <hyperlink ref="D23" r:id="rId44" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{79C6B99F-3134-484C-BF17-FF032736A4F6}"/>
+    <hyperlink ref="C25" r:id="rId45" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{F6E541ED-A56D-4990-98EC-140DB39C69BA}"/>
+    <hyperlink ref="D25" r:id="rId46" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{A0CF9FAE-BAE8-4388-B3DA-F87DE7AAD9AE}"/>
+    <hyperlink ref="C27" r:id="rId47" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{FE8FBBD9-8143-413A-8354-C1249A1B80F8}"/>
+    <hyperlink ref="D27" r:id="rId48" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{8C4BE03A-3602-4A55-A11A-8786FAAD6358}"/>
+    <hyperlink ref="D2" r:id="rId49" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{6E419829-2BDF-4BBE-A274-10468CF12194}"/>
+    <hyperlink ref="C2" r:id="rId50" display="\\DataSet\\TL_DataSet\\BaseRates_GSFile\\" xr:uid="{1044188A-0CC2-46A6-AF0B-7E0E318E3BBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId49"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId51"/>
 </worksheet>
 </file>
 

</xml_diff>